<commit_message>
Added custom view ClearEditText
</commit_message>
<xml_diff>
--- a/return_visitor_v5_ui_flow.xlsx
+++ b/return_visitor_v5_ui_flow.xlsx
@@ -2832,14 +2832,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>134717</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -2849,7 +2849,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="342900" y="9886950"/>
+          <a:off x="371475" y="7696200"/>
           <a:ext cx="2124075" cy="325217"/>
           <a:chOff x="4191000" y="2095500"/>
           <a:chExt cx="2124075" cy="325217"/>
@@ -2970,685 +2970,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="94" name="グループ化 93"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="352425" y="7705724"/>
-          <a:ext cx="2124075" cy="1743075"/>
-          <a:chOff x="352425" y="7705724"/>
-          <a:chExt cx="2124075" cy="1743075"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="91" name="グループ化 90"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="352425" y="7705724"/>
-            <a:ext cx="2124075" cy="1743075"/>
-            <a:chOff x="352425" y="8181974"/>
-            <a:chExt cx="2124075" cy="1743075"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="81" name="角丸四角形 80"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="352425" y="8181974"/>
-              <a:ext cx="2124075" cy="1743075"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst>
-                <a:gd name="adj" fmla="val 2254"/>
-              </a:avLst>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>　　四伊清司　男 </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>31</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>～</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>40</a:t>
-              </a:r>
-              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="83" name="円/楕円 82"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="438150" y="8296275"/>
-              <a:ext cx="133350" cy="133350"/>
-            </a:xfrm>
-            <a:prstGeom prst="ellipse">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="92D050"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="84" name="テキスト ボックス 83"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="380999" y="8391526"/>
-              <a:ext cx="866775" cy="247650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                  <a:solidFill>
-                    <a:srgbClr val="0070C0"/>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>会えた　スイッチ</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="85" name="テキスト ボックス 84"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="380999" y="8763001"/>
-              <a:ext cx="866775" cy="247650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                  <a:solidFill>
-                    <a:srgbClr val="0070C0"/>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>配布物</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="86" name="テキスト ボックス 85"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="390524" y="8934451"/>
-              <a:ext cx="866775" cy="247650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                  <a:solidFill>
-                    <a:srgbClr val="0070C0"/>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>タグ</a:t>
-              </a:r>
-              <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="87" name="テキスト ボックス 86"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="390524" y="9096376"/>
-              <a:ext cx="1104901" cy="247650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                  <a:solidFill>
-                    <a:srgbClr val="0070C0"/>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>次回訪問の優先度</a:t>
-              </a:r>
-              <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="88" name="テキスト ボックス 87"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="390524" y="9267826"/>
-              <a:ext cx="1104901" cy="247650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                  <a:solidFill>
-                    <a:srgbClr val="0070C0"/>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>メモ</a:t>
-              </a:r>
-              <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="89" name="テキスト ボックス 88"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="400049" y="9439276"/>
-              <a:ext cx="1104901" cy="247650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                  <a:solidFill>
-                    <a:srgbClr val="0070C0"/>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>再訪問としてカウント</a:t>
-              </a:r>
-              <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="90" name="テキスト ボックス 89"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="409574" y="9610726"/>
-              <a:ext cx="1104901" cy="247650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                  <a:solidFill>
-                    <a:srgbClr val="0070C0"/>
-                  </a:solidFill>
-                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                </a:rPr>
-                <a:t>研究としてカウント</a:t>
-              </a:r>
-              <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-            <a:p>
-              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="92" name="テキスト ボックス 91"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="371476" y="8105775"/>
-            <a:ext cx="790574" cy="247650"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              </a:rPr>
-              <a:t>情報の編集</a:t>
-            </a:r>
-            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3657,7 +2987,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="342900" y="9553575"/>
+          <a:off x="342900" y="9944100"/>
           <a:ext cx="2124075" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -3709,65 +3039,734 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>209549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="95" name="テキスト ボックス 94"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="グループ化 2"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1704975" y="7905749"/>
-          <a:ext cx="714375" cy="247650"/>
+          <a:off x="352425" y="8096249"/>
+          <a:ext cx="2124075" cy="1743075"/>
+          <a:chOff x="352425" y="8096249"/>
+          <a:chExt cx="2124075" cy="1743075"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="94" name="グループ化 93"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="352425" y="8096249"/>
+            <a:ext cx="2124075" cy="1743075"/>
+            <a:chOff x="352425" y="7705724"/>
+            <a:chExt cx="2124075" cy="1743075"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="91" name="グループ化 90"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="352425" y="7705724"/>
+              <a:ext cx="2124075" cy="1743075"/>
+              <a:chOff x="352425" y="8181974"/>
+              <a:chExt cx="2124075" cy="1743075"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="81" name="角丸四角形 80"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="352425" y="8181974"/>
+                <a:ext cx="2124075" cy="1743075"/>
+              </a:xfrm>
+              <a:prstGeom prst="roundRect">
+                <a:avLst>
+                  <a:gd name="adj" fmla="val 2254"/>
+                </a:avLst>
+              </a:prstGeom>
+              <a:noFill/>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>　　四伊清司　男 </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>31</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>～</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>40</a:t>
+                </a:r>
+                <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="83" name="円/楕円 82"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="438150" y="8296275"/>
+                <a:ext cx="133350" cy="133350"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
-              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
-            </a:rPr>
-            <a:t>開閉スイッチ</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="84" name="テキスト ボックス 83"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="380999" y="8391526"/>
+                <a:ext cx="866775" cy="247650"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                    <a:solidFill>
+                      <a:srgbClr val="0070C0"/>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>会えた　スイッチ</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="85" name="テキスト ボックス 84"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="380999" y="8763001"/>
+                <a:ext cx="866775" cy="247650"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                    <a:solidFill>
+                      <a:srgbClr val="0070C0"/>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>配布物</a:t>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="86" name="テキスト ボックス 85"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="390524" y="8934451"/>
+                <a:ext cx="866775" cy="247650"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                    <a:solidFill>
+                      <a:srgbClr val="0070C0"/>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>タグ</a:t>
+                </a:r>
+                <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="87" name="テキスト ボックス 86"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="390524" y="9096376"/>
+                <a:ext cx="1104901" cy="247650"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                    <a:solidFill>
+                      <a:srgbClr val="0070C0"/>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>次回訪問の優先度</a:t>
+                </a:r>
+                <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="88" name="テキスト ボックス 87"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="390524" y="9267826"/>
+                <a:ext cx="1104901" cy="247650"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                    <a:solidFill>
+                      <a:srgbClr val="0070C0"/>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>メモ</a:t>
+                </a:r>
+                <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="89" name="テキスト ボックス 88"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="400049" y="9439276"/>
+                <a:ext cx="1104901" cy="247650"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                    <a:solidFill>
+                      <a:srgbClr val="0070C0"/>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>再訪問としてカウント</a:t>
+                </a:r>
+                <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="90" name="テキスト ボックス 89"/>
+              <xdr:cNvSpPr txBox="1"/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="409574" y="9610726"/>
+                <a:ext cx="1104901" cy="247650"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:noFill/>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:scrgbClr r="0" g="0" b="0"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+                <a:noAutofit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                    <a:solidFill>
+                      <a:srgbClr val="0070C0"/>
+                    </a:solidFill>
+                    <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                    <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  </a:rPr>
+                  <a:t>研究としてカウント</a:t>
+                </a:r>
+                <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:endParaRPr>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="92" name="テキスト ボックス 91"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="371476" y="8105775"/>
+              <a:ext cx="790574" cy="247650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:rPr>
+                <a:t>情報の編集</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="95" name="テキスト ボックス 94"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1704975" y="8324849"/>
+            <a:ext cx="714375" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              </a:rPr>
+              <a:t>開閉スイッチ</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4060,10 +4059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI100"/>
+  <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="T47" sqref="T47"/>
+      <selection activeCell="Y45" sqref="Y45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.15"/>

</xml_diff>